<commit_message>
Echo für eigene Nachrichten in MQTT unterbunden+MQTT senden von files möglich+Verschiede Subs möglich+Room-String erstellt(derzeitig deaktiviert, da sonst keine Verbindung zum Hochschulbroker möglich ist)+Scoreboard Activity erstellt+Beschreibung zum Einbinden in README.md eingefuegt+Nearfly-Listener minimiert+Code aufgeräumt+Sichbarkeiten von Klassen geändert+Scoreboard Activity Bugfix+forwardExecutor vorzeitig verändert
</commit_message>
<xml_diff>
--- a/Diagramme/AnforderungsmatrixNew.xlsx
+++ b/Diagramme/AnforderungsmatrixNew.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AcerPredator\Desktop\20thesis04\Diagramme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99C7795-8E77-42E4-81F5-3600ABF06BA6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746ED000-2DED-48DE-8911-CF88FB7701F6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F33CD82C-E8A6-4469-983D-9B83A8EFDD79}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="19">
   <si>
     <t>Messenger</t>
   </si>
@@ -45,15 +45,9 @@
     <t>Die Nachrichten müssen den Absender enthalten</t>
   </si>
   <si>
-    <t>funktionale Anforderungen</t>
-  </si>
-  <si>
     <t>Text Nachrichten senden</t>
   </si>
   <si>
-    <t>Bildnachrichten senden</t>
-  </si>
-  <si>
     <t>Priorisierung der Nachrichtentypen</t>
   </si>
   <si>
@@ -63,22 +57,12 @@
     <t>Echtzeitfähigkeit für ein flüssiges Multiplayer-Spiel-Verfalten bei 30 FPS pro Spieler</t>
   </si>
   <si>
-    <t>erkennbare Anforderungen</t>
-  </si>
-  <si>
-    <t>extrapoliert</t>
-  </si>
-  <si>
     <t>Möglichkeit konfigurierbar Nachrichten zeitgleich zu empfangen, auch wenn verzögert</t>
   </si>
   <si>
     <t>Sichtbarkeit der Nachrichten nur innerhalb derselben App</t>
   </si>
   <si>
-    <t xml:space="preserve">Das System soll dem Entwickler die Möglichkeit geben, die höchste auftretenden Round-Trip Time während des Betriebes zu messen.
-</t>
-  </si>
-  <si>
     <t>Das System muss dem Nutzer die Möglichkeit geben, zu entscheide ob bei Verbindungsabbruch, alle noch nicht versandten Pakete bis zur wiederhergestellten Verbindung gehalten oder verworfen werden sollen</t>
   </si>
   <si>
@@ -89,6 +73,15 @@
   </si>
   <si>
     <t>Verzögerungsarmes Empfangen der Nachrichten</t>
+  </si>
+  <si>
+    <t>Das System soll dem Entwickler die Möglichkeit geben, die höchste auftretenden Round-Trip Time während des Betriebes zu messen.</t>
+  </si>
+  <si>
+    <t>Multimedia-Nachrichten senden</t>
+  </si>
+  <si>
+    <t>Funktionale Anforderungen</t>
   </si>
 </sst>
 </file>
@@ -120,7 +113,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -147,19 +140,6 @@
       <left style="thin">
         <color theme="2" tint="-0.499984740745262"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color theme="2" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.499984740745262"/>
-      </left>
       <right style="thin">
         <color theme="2" tint="-0.499984740745262"/>
       </right>
@@ -302,9 +282,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -313,43 +293,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -669,230 +643,207 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.5703125" style="3" customWidth="1"/>
-    <col min="3" max="6" width="3.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.85546875" style="3" customWidth="1"/>
+    <col min="2" max="6" width="3.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="129" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4"/>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="B2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="10"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="12"/>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="12"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="13" t="s">
+      <c r="B13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="A11:A14"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>